<commit_message>
Cleaning of branch and adding of script for combining dataframes
</commit_message>
<xml_diff>
--- a/COINs Intelektuellen-Ranking.xlsx
+++ b/COINs Intelektuellen-Ranking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{2268F253-0306-46AB-8634-3E5BB2888913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C9DBFDF-5D2D-461B-9156-4C329E20F41A}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="3540" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27615" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -1399,7 +1399,7 @@
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000AEB9A43}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1436,7 @@
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000D5779E16}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1473,7 +1473,7 @@
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E61A23C}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1510,7 +1510,7 @@
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A7CB522}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1547,7 +1547,7 @@
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000BBB7B622}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1805,8 +1805,8 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>